<commit_message>
amox + clav acid with PAI
</commit_message>
<xml_diff>
--- a/Data As Is/EST/Import-amoxicillin-clavulanicAcid-packages-2023-06-20.xlsx
+++ b/Data As Is/EST/Import-amoxicillin-clavulanicAcid-packages-2023-06-20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Standardimine\UNICOM\Ravimid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA72E49B-4D72-41FC-BFB4-91510CFE59C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF43200-CDEA-45F1-9D61-ECF846743FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="180">
   <si>
     <t>Müügiloa number</t>
   </si>
@@ -226,9 +226,6 @@
     <t>Süste-/infusioonilahus</t>
   </si>
   <si>
-    <t>1g+0,2g</t>
-  </si>
-  <si>
     <t>1g, 0.2g</t>
   </si>
   <si>
@@ -289,9 +286,6 @@
     <t>Suukaudne suspensioon</t>
   </si>
   <si>
-    <t>11,4mg+80mg/1ml</t>
-  </si>
-  <si>
     <t>11.4mg/ml, 80mg/ml</t>
   </si>
   <si>
@@ -331,9 +325,6 @@
     <t>1660474</t>
   </si>
   <si>
-    <t>200mg+1000mg</t>
-  </si>
-  <si>
     <t>200mg, 1000mg</t>
   </si>
   <si>
@@ -388,9 +379,6 @@
     <t>ORG-100000797</t>
   </si>
   <si>
-    <t>80mg+11,4mg/1ml</t>
-  </si>
-  <si>
     <t>80mg/ml, 11.4mg/ml</t>
   </si>
   <si>
@@ -554,6 +542,27 @@
   </si>
   <si>
     <t>1743971</t>
+  </si>
+  <si>
+    <t>AMOXICILLIN TRIHYDRATE</t>
+  </si>
+  <si>
+    <t>POTASSIUM CLAVULANATE</t>
+  </si>
+  <si>
+    <t>kaaliumklavulanaat, amoksitsilliintrihüdraat</t>
+  </si>
+  <si>
+    <t>amoksitsilliintrihüdraat, kaaliumklavulanaat</t>
+  </si>
+  <si>
+    <t>amoksitsilliinnaatrium, kaaliumklavulanaat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kaaliumklavulanaat, amoksitsilliinnaatrium </t>
+  </si>
+  <si>
+    <t>AMOXICILLIN SODIUM</t>
   </si>
 </sst>
 </file>
@@ -563,7 +572,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -582,6 +591,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -610,13 +626,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -931,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG18"/>
+  <dimension ref="A1:AG21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="P3" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19:T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -942,7 +959,9 @@
     <col min="2" max="2" width="7.90625" customWidth="1"/>
     <col min="3" max="3" width="8.7265625" customWidth="1"/>
     <col min="4" max="4" width="13.08984375" customWidth="1"/>
+    <col min="9" max="9" width="40.90625" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
+    <col min="20" max="20" width="37.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
@@ -1048,7 +1067,7 @@
     </row>
     <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>34</v>
@@ -1057,22 +1076,22 @@
         <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>48</v>
@@ -1081,16 +1100,16 @@
         <v>42</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="N2" s="4">
         <v>44167</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>46</v>
@@ -1102,25 +1121,23 @@
         <v>48</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>121</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="U2" s="3"/>
       <c r="V2" s="3" t="s">
         <v>40</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>40</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>53</v>
@@ -1129,19 +1146,19 @@
         <v>48</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AG2" s="3" t="s">
         <v>48</v>
@@ -1149,7 +1166,7 @@
     </row>
     <row r="3" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>34</v>
@@ -1158,22 +1175,22 @@
         <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>48</v>
@@ -1182,16 +1199,16 @@
         <v>42</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="N3" s="4">
         <v>44321</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>46</v>
@@ -1203,25 +1220,23 @@
         <v>48</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>88</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="U3" s="3"/>
       <c r="V3" s="3" t="s">
         <v>50</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="X3" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="Z3" s="3" t="s">
         <v>53</v>
@@ -1230,19 +1245,19 @@
         <v>48</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="AG3" s="3" t="s">
         <v>48</v>
@@ -1250,7 +1265,7 @@
     </row>
     <row r="4" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>34</v>
@@ -1259,22 +1274,22 @@
         <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>60</v>
@@ -1283,16 +1298,16 @@
         <v>42</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="N4" s="4">
         <v>44649</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>46</v>
@@ -1304,25 +1319,22 @@
         <v>48</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>107</v>
+        <v>176</v>
       </c>
       <c r="V4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Z4" s="3" t="s">
         <v>53</v>
@@ -1337,13 +1349,13 @@
         <v>55</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AG4" s="3" t="s">
         <v>48</v>
@@ -1375,7 +1387,7 @@
         <v>39</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>50</v>
+        <v>177</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>48</v>
@@ -1408,11 +1420,9 @@
         <v>66</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="U5" s="3"/>
       <c r="V5" s="3" t="s">
         <v>40</v>
       </c>
@@ -1423,22 +1433,22 @@
         <v>50</v>
       </c>
       <c r="Y5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="Z5" s="3" t="s">
+      <c r="AA5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AA5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB5" s="3" t="s">
+      <c r="AC5" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AD5" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="AE5" s="3" t="s">
         <v>57</v>
@@ -1452,7 +1462,7 @@
     </row>
     <row r="6" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>34</v>
@@ -1461,22 +1471,22 @@
         <v>35</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>60</v>
@@ -1485,16 +1495,16 @@
         <v>42</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="N6" s="4">
         <v>36042</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>46</v>
@@ -1506,14 +1516,12 @@
         <v>48</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="U6" s="3"/>
       <c r="V6" s="3" t="s">
         <v>40</v>
       </c>
@@ -1524,7 +1532,7 @@
         <v>50</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>53</v>
@@ -1539,13 +1547,13 @@
         <v>55</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="AE6" s="3" t="s">
         <v>57</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="AG6" s="3" t="s">
         <v>48</v>
@@ -1553,7 +1561,7 @@
     </row>
     <row r="7" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>34</v>
@@ -1562,7 +1570,7 @@
         <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>36</v>
@@ -1571,13 +1579,13 @@
         <v>51</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>60</v>
@@ -1595,7 +1603,7 @@
         <v>36980</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>46</v>
@@ -1607,14 +1615,12 @@
         <v>48</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U7" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="U7" s="3"/>
       <c r="V7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1654,7 +1660,7 @@
     </row>
     <row r="8" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>34</v>
@@ -1663,22 +1669,22 @@
         <v>35</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>48</v>
@@ -1696,7 +1702,7 @@
         <v>36980</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>46</v>
@@ -1708,25 +1714,23 @@
         <v>48</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>88</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="U8" s="3"/>
       <c r="V8" s="3" t="s">
         <v>50</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="X8" s="3" t="s">
         <v>40</v>
       </c>
       <c r="Y8" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Z8" s="3" t="s">
         <v>53</v>
@@ -1735,13 +1739,13 @@
         <v>48</v>
       </c>
       <c r="AB8" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AD8" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AE8" s="3" t="s">
         <v>57</v>
@@ -1755,7 +1759,7 @@
     </row>
     <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>34</v>
@@ -1764,22 +1768,22 @@
         <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>41</v>
@@ -1797,7 +1801,7 @@
         <v>36980</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>46</v>
@@ -1809,25 +1813,23 @@
         <v>48</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U9" s="3" t="s">
-        <v>79</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="U9" s="3"/>
       <c r="V9" s="3" t="s">
         <v>50</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X9" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Z9" s="3" t="s">
         <v>53</v>
@@ -1856,7 +1858,7 @@
     </row>
     <row r="10" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>34</v>
@@ -1865,22 +1867,22 @@
         <v>35</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>60</v>
@@ -1898,7 +1900,7 @@
         <v>36980</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>46</v>
@@ -1910,25 +1912,23 @@
         <v>48</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U10" s="3" t="s">
-        <v>79</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="U10" s="3"/>
       <c r="V10" s="3" t="s">
         <v>50</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X10" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Z10" s="3" t="s">
         <v>53</v>
@@ -1981,7 +1981,7 @@
         <v>39</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>60</v>
@@ -2014,11 +2014,9 @@
         <v>49</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U11" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="U11" s="3"/>
       <c r="V11" s="3" t="s">
         <v>40</v>
       </c>
@@ -2058,7 +2056,7 @@
     </row>
     <row r="12" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>34</v>
@@ -2067,13 +2065,13 @@
         <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>64</v>
@@ -2082,7 +2080,7 @@
         <v>39</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>48</v>
@@ -2091,16 +2089,16 @@
         <v>42</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="N12" s="4">
         <v>41033</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="P12" s="3" t="s">
         <v>46</v>
@@ -2115,43 +2113,41 @@
         <v>66</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>102</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="U12" s="3"/>
       <c r="V12" s="3" t="s">
         <v>50</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="X12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AA12" s="3" t="s">
         <v>48</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AD12" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AE12" s="3" t="s">
         <v>57</v>
       </c>
       <c r="AF12" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="AG12" s="3" t="s">
         <v>48</v>
@@ -2159,7 +2155,7 @@
     </row>
     <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>34</v>
@@ -2168,22 +2164,22 @@
         <v>35</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>60</v>
@@ -2192,16 +2188,16 @@
         <v>42</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N13" s="4">
         <v>42069</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>46</v>
@@ -2213,14 +2209,12 @@
         <v>48</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="U13" s="3"/>
       <c r="V13" s="3" t="s">
         <v>40</v>
       </c>
@@ -2231,7 +2225,7 @@
         <v>50</v>
       </c>
       <c r="Y13" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Z13" s="3" t="s">
         <v>53</v>
@@ -2240,7 +2234,7 @@
         <v>48</v>
       </c>
       <c r="AB13" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AC13" s="3" t="s">
         <v>55</v>
@@ -2252,7 +2246,7 @@
         <v>57</v>
       </c>
       <c r="AF13" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AG13" s="3" t="s">
         <v>48</v>
@@ -2260,7 +2254,7 @@
     </row>
     <row r="14" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>34</v>
@@ -2269,22 +2263,22 @@
         <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>60</v>
@@ -2293,16 +2287,16 @@
         <v>42</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="N14" s="4">
         <v>42263</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="P14" s="3" t="s">
         <v>46</v>
@@ -2314,14 +2308,12 @@
         <v>48</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U14" s="3" t="s">
-        <v>51</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="U14" s="3"/>
       <c r="V14" s="3" t="s">
         <v>40</v>
       </c>
@@ -2332,7 +2324,7 @@
         <v>50</v>
       </c>
       <c r="Y14" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Z14" s="3" t="s">
         <v>53</v>
@@ -2344,16 +2336,16 @@
         <v>54</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="AD14" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AE14" s="3" t="s">
         <v>57</v>
       </c>
       <c r="AF14" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="AG14" s="3" t="s">
         <v>48</v>
@@ -2361,7 +2353,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>34</v>
@@ -2370,22 +2362,22 @@
         <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>60</v>
@@ -2394,16 +2386,16 @@
         <v>42</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="N15" s="4">
         <v>42682</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>46</v>
@@ -2415,14 +2407,12 @@
         <v>48</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U15" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="U15" s="3"/>
       <c r="V15" s="3" t="s">
         <v>40</v>
       </c>
@@ -2442,19 +2432,19 @@
         <v>48</v>
       </c>
       <c r="AB15" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AC15" s="3" t="s">
         <v>55</v>
       </c>
       <c r="AD15" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="AE15" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AF15" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AG15" s="3" t="s">
         <v>48</v>
@@ -2462,7 +2452,7 @@
     </row>
     <row r="16" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>34</v>
@@ -2471,22 +2461,22 @@
         <v>35</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>48</v>
@@ -2495,16 +2485,16 @@
         <v>42</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="N16" s="4">
         <v>42801</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="P16" s="3" t="s">
         <v>46</v>
@@ -2516,25 +2506,22 @@
         <v>48</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U16" s="3" t="s">
-        <v>88</v>
+        <v>176</v>
       </c>
       <c r="V16" s="3" t="s">
         <v>50</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="X16" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Y16" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="Z16" s="3" t="s">
         <v>53</v>
@@ -2543,19 +2530,19 @@
         <v>48</v>
       </c>
       <c r="AB16" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="AC16" s="3" t="s">
         <v>48</v>
       </c>
       <c r="AD16" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AE16" s="3" t="s">
         <v>57</v>
       </c>
       <c r="AF16" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AG16" s="3" t="s">
         <v>48</v>
@@ -2563,7 +2550,7 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>34</v>
@@ -2572,22 +2559,22 @@
         <v>35</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>48</v>
@@ -2596,16 +2583,16 @@
         <v>42</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="N17" s="4">
         <v>42990</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>46</v>
@@ -2617,25 +2604,23 @@
         <v>48</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U17" s="3" t="s">
-        <v>121</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="U17" s="3"/>
       <c r="V17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="X17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="Y17" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Z17" s="3" t="s">
         <v>53</v>
@@ -2644,19 +2629,19 @@
         <v>48</v>
       </c>
       <c r="AB17" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="AC17" s="3" t="s">
         <v>48</v>
       </c>
       <c r="AD17" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AE17" s="3" t="s">
         <v>57</v>
       </c>
       <c r="AF17" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AG17" s="3" t="s">
         <v>48</v>
@@ -2664,7 +2649,7 @@
     </row>
     <row r="18" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>34</v>
@@ -2673,22 +2658,22 @@
         <v>35</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>51</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>60</v>
@@ -2697,16 +2682,16 @@
         <v>42</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="N18" s="4">
         <v>43354</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="P18" s="3" t="s">
         <v>46</v>
@@ -2718,13 +2703,10 @@
         <v>48</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U18" s="3" t="s">
-        <v>51</v>
+        <v>176</v>
       </c>
       <c r="V18" s="3" t="s">
         <v>50</v>
@@ -2736,7 +2718,7 @@
         <v>50</v>
       </c>
       <c r="Y18" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Z18" s="3" t="s">
         <v>53</v>
@@ -2745,22 +2727,37 @@
         <v>48</v>
       </c>
       <c r="AB18" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="AC18" s="3" t="s">
         <v>55</v>
       </c>
       <c r="AD18" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="AE18" s="3" t="s">
         <v>57</v>
       </c>
       <c r="AF18" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AG18" s="3" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="T19" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="T20" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="T21" s="6" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filled in the gaps in table
</commit_message>
<xml_diff>
--- a/Data As Is/EST/Import-amoxicillin-clavulanicAcid-packages-2023-06-20.xlsx
+++ b/Data As Is/EST/Import-amoxicillin-clavulanicAcid-packages-2023-06-20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Standardimine\UNICOM\Ravimid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF43200-CDEA-45F1-9D61-ECF846743FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA9327E-6FA2-4D05-BCEC-4E97B333A321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Otsing" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Otsing!$A$1:$AG$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Otsing!$A$1:$AH$18</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="176">
   <si>
     <t>Müügiloa number</t>
   </si>
@@ -211,9 +211,6 @@
     <t>149896</t>
   </si>
   <si>
-    <t>1017694</t>
-  </si>
-  <si>
     <t>0.2g+1g</t>
   </si>
   <si>
@@ -436,24 +433,15 @@
     <t>LOC-100023139</t>
   </si>
   <si>
-    <t>1718333</t>
-  </si>
-  <si>
     <t>1013820</t>
   </si>
   <si>
-    <t>1822700</t>
-  </si>
-  <si>
     <t>7713</t>
   </si>
   <si>
     <t>1029021</t>
   </si>
   <si>
-    <t>1840722</t>
-  </si>
-  <si>
     <t>8062</t>
   </si>
   <si>
@@ -526,9 +514,6 @@
     <t>933817</t>
   </si>
   <si>
-    <t>1701155</t>
-  </si>
-  <si>
     <t>5596</t>
   </si>
   <si>
@@ -538,18 +523,9 @@
     <t>Hoida temperatuuril kuni 25°C, Hoida originaalpakendis</t>
   </si>
   <si>
-    <t>1345407</t>
-  </si>
-  <si>
     <t>1743971</t>
   </si>
   <si>
-    <t>AMOXICILLIN TRIHYDRATE</t>
-  </si>
-  <si>
-    <t>POTASSIUM CLAVULANATE</t>
-  </si>
-  <si>
     <t>kaaliumklavulanaat, amoksitsilliintrihüdraat</t>
   </si>
   <si>
@@ -562,7 +538,19 @@
     <t xml:space="preserve">kaaliumklavulanaat, amoksitsilliinnaatrium </t>
   </si>
   <si>
-    <t>AMOXICILLIN SODIUM</t>
+    <t>1 Pudel</t>
+  </si>
+  <si>
+    <t>70 ml</t>
+  </si>
+  <si>
+    <t>5 Viaal</t>
+  </si>
+  <si>
+    <t>Sisepakendi suurus</t>
+  </si>
+  <si>
+    <t>10 Viaal</t>
   </si>
 </sst>
 </file>
@@ -948,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG21"/>
+  <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P3" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19:T21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19:U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -959,12 +947,16 @@
     <col min="2" max="2" width="7.90625" customWidth="1"/>
     <col min="3" max="3" width="8.7265625" customWidth="1"/>
     <col min="4" max="4" width="13.08984375" customWidth="1"/>
+    <col min="6" max="6" width="6.54296875" customWidth="1"/>
+    <col min="7" max="7" width="8.26953125" customWidth="1"/>
+    <col min="8" max="8" width="6.81640625" customWidth="1"/>
     <col min="9" max="9" width="40.90625" customWidth="1"/>
-    <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="20" max="20" width="37.1796875" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
+    <col min="19" max="19" width="26.26953125" customWidth="1"/>
+    <col min="21" max="21" width="37.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -996,78 +988,81 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>34</v>
@@ -1075,98 +1070,101 @@
       <c r="C2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>139</v>
+      <c r="D2" s="3">
+        <v>1822700</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>48</v>
+        <v>171</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="N2" s="4">
+      <c r="O2" s="4">
         <v>44167</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="P2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="S2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="AB2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE2" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="AC2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AF2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>34</v>
@@ -1174,98 +1172,101 @@
       <c r="C3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>142</v>
+      <c r="D3" s="3">
+        <v>1840722</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>48</v>
+        <v>171</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="O3" s="4">
+        <v>44321</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG3" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="N3" s="4">
-        <v>44321</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>34</v>
@@ -1274,94 +1275,94 @@
         <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="O4" s="4">
+        <v>44649</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="N4" s="4">
-        <v>44649</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE4" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AF4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>61</v>
       </c>
@@ -1371,98 +1372,99 @@
       <c r="C5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>62</v>
+      <c r="D5" s="3">
+        <v>1017694</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K5" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="N5" s="4">
+      <c r="O5" s="4">
         <v>35363</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S5" s="3" t="s">
+      <c r="U5" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y5" s="3" t="s">
+      <c r="AA5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="Z5" s="3" t="s">
+      <c r="AB5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="AA5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB5" s="3" t="s">
+      <c r="AD5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AE5" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AD5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE5" s="3" t="s">
+      <c r="AF5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AF5" s="3" t="s">
+      <c r="AG5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AG5" s="3" t="s">
+      <c r="AH5" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>34</v>
@@ -1471,97 +1473,98 @@
         <v>35</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="3"/>
+      <c r="L6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="N6" s="4">
+      <c r="O6" s="4">
         <v>36042</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="P6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="R6" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="S6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="X6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="X6" s="3" t="s">
+      <c r="Y6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="Y6" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="Z6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA6" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="AB6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AD6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AD6" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="AE6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AF6" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="AG6" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH6" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>34</v>
@@ -1570,7 +1573,7 @@
         <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>36</v>
@@ -1579,88 +1582,89 @@
         <v>51</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="N7" s="4">
+      <c r="O7" s="4">
         <v>36980</v>
       </c>
-      <c r="O7" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="P7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="R7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="R7" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="S7" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="W7" s="3" t="s">
+      <c r="X7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="X7" s="3" t="s">
+      <c r="Y7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Y7" s="3" t="s">
+      <c r="Z7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Z7" s="3" t="s">
+      <c r="AA7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA7" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="AB7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AC7" s="3" t="s">
+      <c r="AD7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AD7" s="3" t="s">
+      <c r="AE7" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AE7" s="3" t="s">
+      <c r="AF7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AF7" s="3" t="s">
+      <c r="AG7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AG7" s="3" t="s">
+      <c r="AH7" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>34</v>
@@ -1669,97 +1673,98 @@
         <v>35</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="N8" s="4">
+      <c r="O8" s="4">
         <v>36980</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="P8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="T8" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S8" s="3" t="s">
+      <c r="U8" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z8" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="T8" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="X8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y8" s="3" t="s">
+      <c r="AA8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC8" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Z8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB8" s="3" t="s">
+      <c r="AD8" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="AC8" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD8" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="AE8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AF8" s="3" t="s">
+      <c r="AG8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AG8" s="3" t="s">
+      <c r="AH8" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>34</v>
@@ -1768,97 +1773,98 @@
         <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="3"/>
+      <c r="L9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="N9" s="4">
+      <c r="O9" s="4">
         <v>36980</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="P9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z9" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="P9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="X9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y9" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z9" s="3" t="s">
+      <c r="AA9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA9" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="AB9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AC9" s="3" t="s">
+      <c r="AD9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AD9" s="3" t="s">
+      <c r="AE9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AE9" s="3" t="s">
+      <c r="AF9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AF9" s="3" t="s">
+      <c r="AG9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AG9" s="3" t="s">
+      <c r="AH9" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>34</v>
@@ -1867,95 +1873,96 @@
         <v>35</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="3"/>
+      <c r="L10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="N10" s="4">
+      <c r="O10" s="4">
         <v>36980</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="P10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="P10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W10" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="X10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y10" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z10" s="3" t="s">
+      <c r="AA10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA10" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="AB10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AC10" s="3" t="s">
+      <c r="AD10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AD10" s="3" t="s">
+      <c r="AE10" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AE10" s="3" t="s">
+      <c r="AF10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AF10" s="3" t="s">
+      <c r="AG10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AG10" s="3" t="s">
+      <c r="AH10" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -1981,82 +1988,83 @@
         <v>39</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="3"/>
+      <c r="L11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="N11" s="4">
+      <c r="O11" s="4">
         <v>38954</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="P11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="Q11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="R11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="R11" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="S11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="T11" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3" t="s">
+      <c r="U11" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="W11" s="3" t="s">
+      <c r="X11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="X11" s="3" t="s">
+      <c r="Y11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Y11" s="3" t="s">
+      <c r="Z11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Z11" s="3" t="s">
+      <c r="AA11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA11" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="AB11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AC11" s="3" t="s">
+      <c r="AD11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AD11" s="3" t="s">
+      <c r="AE11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AE11" s="3" t="s">
+      <c r="AF11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AF11" s="3" t="s">
+      <c r="AG11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AG11" s="3" t="s">
+      <c r="AH11" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>34</v>
@@ -2064,98 +2072,99 @@
       <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>171</v>
+      <c r="D12" s="3">
+        <v>1345407</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="M12" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="N12" s="4">
+        <v>151</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="O12" s="4">
         <v>41033</v>
       </c>
-      <c r="O12" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="P12" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="R12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="R12" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="S12" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="W12" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="X12" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Y12" s="3" t="s">
+      <c r="Z12" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="Z12" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB12" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="AC12" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD12" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE12" s="3" t="s">
+      <c r="AF12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AF12" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="AG12" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="AH12" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>34</v>
@@ -2164,97 +2173,98 @@
         <v>35</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="3"/>
+      <c r="L13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="M13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="N13" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="O13" s="4">
+        <v>42069</v>
+      </c>
+      <c r="P13" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="N13" s="4">
-        <v>42069</v>
-      </c>
-      <c r="O13" s="3" t="s">
+      <c r="Q13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z13" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="P13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y13" s="3" t="s">
+      <c r="AA13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC13" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="Z13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB13" s="3" t="s">
+      <c r="AD13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG13" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="AC13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF13" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="AG13" s="3" t="s">
+      <c r="AH13" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>34</v>
@@ -2263,97 +2273,98 @@
         <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="K14" s="3"/>
+      <c r="L14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="M14" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O14" s="4">
+        <v>42263</v>
+      </c>
+      <c r="P14" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="N14" s="4">
-        <v>42263</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="P14" s="3" t="s">
+      <c r="Q14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q14" s="3" t="s">
+      <c r="R14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="R14" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="S14" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="W14" s="3" t="s">
+      <c r="X14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="X14" s="3" t="s">
+      <c r="Y14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="Y14" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="Z14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA14" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="AB14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AC14" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="AD14" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="AE14" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AF14" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="AG14" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AH14" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>34</v>
@@ -2362,97 +2373,98 @@
         <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="3"/>
+      <c r="L15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="M15" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N15" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="M15" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="N15" s="4">
+      <c r="O15" s="4">
         <v>42682</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="P15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC15" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="P15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="T15" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="X15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB15" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC15" s="3" t="s">
+      <c r="AD15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AD15" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="AE15" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG15" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AF15" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AG15" s="3" t="s">
+      <c r="AH15" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>34</v>
@@ -2460,97 +2472,100 @@
       <c r="C16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>167</v>
+      <c r="D16" s="3">
+        <v>1701155</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>48</v>
+        <v>171</v>
       </c>
       <c r="K16" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O16" s="4">
+        <v>42801</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC16" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE16" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG16" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="M16" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="N16" s="4">
-        <v>42801</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S16" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="V16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W16" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="X16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y16" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB16" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="AC16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD16" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF16" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AG16" s="3" t="s">
+      <c r="AH16" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>34</v>
@@ -2558,98 +2573,101 @@
       <c r="C17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>137</v>
+      <c r="D17" s="3">
+        <v>1718333</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>48</v>
+        <v>171</v>
       </c>
       <c r="K17" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="M17" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N17" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="O17" s="4">
+        <v>42990</v>
+      </c>
+      <c r="P17" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="N17" s="4">
-        <v>42990</v>
-      </c>
-      <c r="O17" s="3" t="s">
+      <c r="Q17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X17" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC17" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE17" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG17" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="P17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="T17" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="W17" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="X17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y17" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB17" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AC17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD17" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE17" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF17" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="AG17" s="3" t="s">
+      <c r="AH17" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>34</v>
@@ -2658,115 +2676,109 @@
         <v>35</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>51</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="M18" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O18" s="4">
+        <v>43354</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z18" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC18" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE18" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AF18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG18" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="M18" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="N18" s="4">
-        <v>43354</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S18" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="T18" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="V18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="X18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y18" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB18" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="AC18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD18" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="AE18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF18" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AG18" s="3" t="s">
+      <c r="AH18" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="T19" s="3" t="s">
-        <v>179</v>
-      </c>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="U19" s="3"/>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="T20" s="6" t="s">
-        <v>173</v>
-      </c>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="U20" s="6"/>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="T21" s="6" t="s">
-        <v>174</v>
-      </c>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="U21" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG18" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AG18">
+  <autoFilter ref="A1:AH18" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH18">
       <sortCondition ref="A1:A18"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AG18">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH18">
     <sortCondition ref="E1:E18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>